<commit_message>
CN0611: Escaleta con ajuste
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion11/Escaleta_CN_06_11_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion11/Escaleta_CN_06_11_CO.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="15" yWindow="90" windowWidth="10740" windowHeight="11580"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="201">
   <si>
     <t>Asignatura</t>
   </si>
@@ -548,9 +548,6 @@
     <t>Actividad que propone un experimento para estudiar el movimiento de los cuerpos y su percepción</t>
   </si>
   <si>
-    <t>MN_3C_24</t>
-  </si>
-  <si>
     <t>La fuerza de gravedad</t>
   </si>
   <si>
@@ -624,6 +621,12 @@
   </si>
   <si>
     <t>m101a</t>
+  </si>
+  <si>
+    <t>3C</t>
+  </si>
+  <si>
+    <t>La fuerza de la gravedad</t>
   </si>
 </sst>
 </file>
@@ -674,7 +677,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -723,6 +726,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="39">
     <border>
@@ -1221,7 +1230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1315,6 +1324,12 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1330,12 +1345,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1609,7 +1621,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1622,8 +1634,8 @@
   </sheetPr>
   <dimension ref="A1:U95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X30" sqref="X30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,94 +1664,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="71" t="s">
+      <c r="G1" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="71" t="s">
+      <c r="H1" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="71" t="s">
+      <c r="I1" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="71" t="s">
+      <c r="J1" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="71" t="s">
+      <c r="K1" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="74" t="s">
+      <c r="L1" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="73" t="s">
+      <c r="M1" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="73"/>
-      <c r="O1" s="71" t="s">
+      <c r="N1" s="79"/>
+      <c r="O1" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="71" t="s">
+      <c r="P1" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="71" t="s">
+      <c r="Q1" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="71" t="s">
+      <c r="R1" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="71" t="s">
+      <c r="S1" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="71" t="s">
+      <c r="T1" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="71" t="s">
+      <c r="U1" s="77" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="20" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="75"/>
+      <c r="A2" s="78"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="81"/>
       <c r="M2" s="19" t="s">
         <v>86</v>
       </c>
       <c r="N2" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="72"/>
-      <c r="R2" s="72"/>
-      <c r="S2" s="72"/>
-      <c r="T2" s="72"/>
-      <c r="U2" s="72"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -1847,7 +1859,7 @@
         <v>138</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="U4" s="39" t="s">
         <v>139</v>
@@ -1867,7 +1879,7 @@
         <v>91</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F5" s="26"/>
       <c r="G5" s="27" t="s">
@@ -1924,7 +1936,7 @@
         <v>91</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F6" s="26"/>
       <c r="G6" s="27" t="s">
@@ -2037,7 +2049,7 @@
       <c r="D8" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="81"/>
+      <c r="E8" s="76"/>
       <c r="F8" s="34"/>
       <c r="G8" s="35" t="s">
         <v>153</v>
@@ -2370,7 +2382,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="77" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>67</v>
       </c>
@@ -2380,7 +2392,7 @@
       <c r="C14" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="76" t="s">
+      <c r="D14" s="71" t="s">
         <v>96</v>
       </c>
       <c r="E14" s="25" t="s">
@@ -2427,7 +2439,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="79" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" s="74" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
         <v>67</v>
       </c>
@@ -2437,7 +2449,7 @@
       <c r="C15" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="78" t="s">
+      <c r="D15" s="73" t="s">
         <v>96</v>
       </c>
       <c r="E15" s="45" t="s">
@@ -2797,7 +2809,7 @@
         <v>119</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H21" s="9">
         <v>19</v>
@@ -2836,7 +2848,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:21" s="77" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>67</v>
       </c>
@@ -2856,7 +2868,7 @@
         <v>119</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H22" s="9">
         <v>20</v>
@@ -2915,7 +2927,7 @@
       </c>
       <c r="F23" s="57"/>
       <c r="G23" s="46" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H23" s="13">
         <v>21</v>
@@ -2968,11 +2980,11 @@
         <v>120</v>
       </c>
       <c r="E24" s="53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H24" s="9">
         <v>22</v>
@@ -2981,7 +2993,7 @@
         <v>19</v>
       </c>
       <c r="J24" s="36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K24" s="37" t="s">
         <v>70</v>
@@ -3025,11 +3037,11 @@
         <v>120</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F25" s="26"/>
       <c r="G25" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H25" s="10">
         <v>23</v>
@@ -3038,7 +3050,7 @@
         <v>19</v>
       </c>
       <c r="J25" s="28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K25" s="29" t="s">
         <v>70</v>
@@ -3052,24 +3064,24 @@
       <c r="P25" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="Q25" s="32">
-        <v>7</v>
-      </c>
-      <c r="R25" s="5" t="s">
+      <c r="Q25" s="82" t="s">
+        <v>199</v>
+      </c>
+      <c r="R25" s="83" t="s">
         <v>135</v>
       </c>
-      <c r="S25" s="5" t="s">
+      <c r="S25" s="83" t="s">
         <v>121</v>
       </c>
-      <c r="T25" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="U25" s="33" t="s">
-        <v>174</v>
+      <c r="T25" s="83" t="s">
+        <v>200</v>
+      </c>
+      <c r="U25" s="84" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:21" s="59" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="80" t="s">
+      <c r="A26" s="75" t="s">
         <v>67</v>
       </c>
       <c r="B26" s="55" t="s">
@@ -3086,7 +3098,7 @@
       </c>
       <c r="F26" s="57"/>
       <c r="G26" s="46" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H26" s="13">
         <v>24</v>
@@ -3095,7 +3107,7 @@
         <v>108</v>
       </c>
       <c r="J26" s="47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K26" s="48" t="s">
         <v>69</v>
@@ -3104,7 +3116,7 @@
         <v>32</v>
       </c>
       <c r="M26" s="58" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N26" s="58"/>
       <c r="O26" s="49"/>
@@ -3121,7 +3133,7 @@
         <v>138</v>
       </c>
       <c r="T26" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="U26" s="51" t="s">
         <v>139</v>
@@ -3143,7 +3155,7 @@
       <c r="E27" s="53"/>
       <c r="F27" s="34"/>
       <c r="G27" s="35" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H27" s="9">
         <v>25</v>
@@ -3152,7 +3164,7 @@
         <v>108</v>
       </c>
       <c r="J27" s="36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K27" s="37" t="s">
         <v>70</v>
@@ -3209,7 +3221,7 @@
         <v>108</v>
       </c>
       <c r="J28" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K28" s="29" t="s">
         <v>70</v>
@@ -3266,7 +3278,7 @@
         <v>108</v>
       </c>
       <c r="J29" s="28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K29" s="29" t="s">
         <v>70</v>
@@ -3314,7 +3326,7 @@
       <c r="E30" s="25"/>
       <c r="F30" s="26"/>
       <c r="G30" s="27" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H30" s="10">
         <v>28</v>
@@ -3323,7 +3335,7 @@
         <v>108</v>
       </c>
       <c r="J30" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K30" s="29" t="s">
         <v>70</v>
@@ -3380,7 +3392,7 @@
         <v>108</v>
       </c>
       <c r="J31" s="28" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K31" s="29" t="s">
         <v>69</v>
@@ -3425,7 +3437,7 @@
         <v>108</v>
       </c>
       <c r="J32" s="28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K32" s="29" t="s">
         <v>69</v>
@@ -3473,7 +3485,7 @@
       <c r="E33" s="25"/>
       <c r="F33" s="26"/>
       <c r="G33" s="27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H33" s="10">
         <v>31</v>
@@ -3482,7 +3494,7 @@
         <v>108</v>
       </c>
       <c r="J33" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K33" s="29" t="s">
         <v>69</v>

</xml_diff>